<commit_message>
need case 3 to be done.
</commit_message>
<xml_diff>
--- a/NewYearChaos/count.xlsx
+++ b/NewYearChaos/count.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
   <si>
     <t>hasil akhir</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>jumped1st</t>
+  </si>
+  <si>
+    <t>countbribes</t>
   </si>
 </sst>
 </file>
@@ -144,12 +147,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -237,16 +240,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -259,9 +298,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q33"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -569,6 +612,9 @@
     <col min="13" max="13" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="6"/>
+    </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>23</v>
@@ -582,7 +628,7 @@
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
       <c r="F2">
@@ -594,7 +640,7 @@
       <c r="H2">
         <v>7</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>8</v>
       </c>
       <c r="J2">
@@ -626,7 +672,7 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>4</v>
       </c>
       <c r="H3">
@@ -652,32 +698,33 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9">
-        <v>3</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="17">
-        <v>4</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="20">
+        <v>4</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="17">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8">
+        <v>7</v>
+      </c>
+      <c r="J4" s="12">
+        <v>7</v>
+      </c>
+      <c r="K4" s="12">
         <v>10</v>
       </c>
+      <c r="L4" s="9"/>
       <c r="N4" t="s">
         <v>6</v>
       </c>
@@ -689,52 +736,86 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="4">
-        <v>8</v>
-      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="18">
+        <v>8</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11">
-        <v>5</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="19">
-        <v>6</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6">
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="21">
+        <v>6</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="19">
         <v>9</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="10">
         <v>9</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="13">
         <v>11</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="13">
         <v>11</v>
       </c>
+      <c r="L6" s="11"/>
       <c r="N6">
         <v>10</v>
       </c>
       <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="16">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
@@ -810,7 +891,7 @@
       <c r="F11">
         <v>4</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H11">
@@ -1014,9 +1095,12 @@
         <v>15</v>
       </c>
     </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="6"/>
+    </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1030,7 +1114,7 @@
       <c r="E23">
         <v>4</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="22">
         <v>5</v>
       </c>
       <c r="G23">
@@ -1054,7 +1138,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1068,7 +1152,7 @@
       <c r="E24">
         <v>6</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="22">
         <v>7</v>
       </c>
       <c r="G24">
@@ -1095,7 +1179,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1106,7 +1190,7 @@
       <c r="E25" t="s">
         <v>4</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="22" t="s">
         <v>4</v>
       </c>
       <c r="G25" t="s">
@@ -1133,15 +1217,16 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1152,7 +1237,7 @@
       <c r="E27" t="s">
         <v>5</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="22" t="s">
         <v>9</v>
       </c>
       <c r="G27" t="s">
@@ -1174,157 +1259,324 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>3</v>
-      </c>
-      <c r="E29">
-        <v>4</v>
-      </c>
-      <c r="F29">
-        <v>5</v>
-      </c>
-      <c r="G29">
-        <v>6</v>
-      </c>
-      <c r="H29">
-        <v>7</v>
-      </c>
-      <c r="I29">
-        <v>8</v>
-      </c>
-      <c r="J29">
-        <v>9</v>
-      </c>
-      <c r="K29">
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
+      </c>
+      <c r="H28">
         <v>10</v>
       </c>
-      <c r="L29">
-        <v>11</v>
+      <c r="I28">
+        <v>12</v>
+      </c>
+      <c r="J28">
+        <v>14</v>
+      </c>
+      <c r="K28">
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30">
         <v>9</v>
       </c>
-      <c r="I30" s="2">
+      <c r="K30">
         <v>10</v>
       </c>
-      <c r="J30" s="3">
-        <v>4</v>
-      </c>
-      <c r="K30">
+      <c r="L30">
         <v>11</v>
-      </c>
-      <c r="L30">
-        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>9</v>
+      </c>
+      <c r="I31" s="2">
+        <v>10</v>
+      </c>
+      <c r="J31" s="3">
+        <v>4</v>
       </c>
       <c r="K31">
-        <v>3</v>
-      </c>
-      <c r="N31" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="L31">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+      <c r="K32">
+        <v>3</v>
+      </c>
+      <c r="N32" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D33">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
         <v>9</v>
       </c>
-      <c r="G33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" t="s">
         <v>10</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>11</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>10</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>11</v>
       </c>
-      <c r="N33">
+      <c r="N34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="6"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <v>7</v>
+      </c>
+      <c r="I37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>7</v>
+      </c>
+      <c r="G38">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="L41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>7</v>
+      </c>
+      <c r="L42">
         <v>15</v>
       </c>
     </row>

</xml_diff>